<commit_message>
amended the pivots for 4phases and 8phases to make calculations for multiple intervals and take the execution spread and PnL data from common files for each interval from SQL query
</commit_message>
<xml_diff>
--- a/results/trend_volatility_results/processed_4phases_data/pivots/pivots_4phases_D1.xlsx
+++ b/results/trend_volatility_results/processed_4phases_data/pivots/pivots_4phases_D1.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,14 +429,13 @@
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="27" customWidth="1" min="3" max="3"/>
     <col width="26" customWidth="1" min="4" max="4"/>
-    <col width="33" customWidth="1" min="5" max="5"/>
-    <col width="35" customWidth="1" min="6" max="6"/>
-    <col width="21" customWidth="1" min="7" max="7"/>
+    <col width="35" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
     <col width="21" customWidth="1" min="8" max="8"/>
-    <col width="21" customWidth="1" min="9" max="9"/>
-    <col width="14" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
-    <col width="31" customWidth="1" min="12" max="12"/>
+    <col width="14" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="31" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -464,40 +463,35 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>weighted_avg_execution_spread_$</t>
+          <t>volume_weighted_avg_spread_in_USD</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>volume_weighted_avg_spread_in_USD</t>
+          <t>PnL_per_lot</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>PnL_per_lot</t>
+          <t>total_profit</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>total_profit</t>
+          <t>pct_total_profit</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>pct_total_profit</t>
+          <t>total_volume</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>total_volume</t>
+          <t>pct_total_volume</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
-        <is>
-          <t>pct_total_volume</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
         <is>
           <t>pct_impact_on_PnL_exec_spread</t>
         </is>
@@ -517,37 +511,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C4" t="n">
-        <v>37.30769230769231</v>
+        <v>36.92307692307693</v>
       </c>
       <c r="D4" t="n">
-        <v>9.208333333330977</v>
+        <v>9.208333333333334</v>
       </c>
       <c r="E4" t="n">
-        <v>8.780303728468926</v>
+        <v>8.40337556322546</v>
       </c>
       <c r="F4" t="n">
-        <v>6.805373247781808</v>
+        <v>-6.240474543628242</v>
       </c>
       <c r="G4" t="n">
-        <v>-6.471519290453474</v>
+        <v>-28378222</v>
       </c>
       <c r="H4" t="n">
-        <v>-29695129.61</v>
+        <v>26.81083570194399</v>
       </c>
       <c r="I4" t="n">
-        <v>28.98532646034216</v>
+        <v>4547446.16</v>
       </c>
       <c r="J4" t="n">
-        <v>4588587.05</v>
+        <v>39.1792541178183</v>
       </c>
       <c r="K4" t="n">
-        <v>39.68290814288032</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.1545232201463356</v>
+        <v>0.1602442238981709</v>
       </c>
     </row>
     <row r="5">
@@ -557,37 +548,34 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C5" t="n">
-        <v>22.69230769230769</v>
+        <v>22.56410256410257</v>
       </c>
       <c r="D5" t="n">
-        <v>9.310344827586329</v>
+        <v>9.310344827586206</v>
       </c>
       <c r="E5" t="n">
-        <v>8.735623008866666</v>
+        <v>8.704009297210991</v>
       </c>
       <c r="F5" t="n">
-        <v>7.516851148941799</v>
+        <v>-23.49091957721433</v>
       </c>
       <c r="G5" t="n">
-        <v>-22.98527659036484</v>
+        <v>-69770150.73</v>
       </c>
       <c r="H5" t="n">
-        <v>-67992421.90000001</v>
+        <v>65.91660492760603</v>
       </c>
       <c r="I5" t="n">
-        <v>66.36719797098127</v>
+        <v>2970090.23</v>
       </c>
       <c r="J5" t="n">
-        <v>2958085.87</v>
+        <v>25.58929029167866</v>
       </c>
       <c r="K5" t="n">
-        <v>25.58204706129792</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.04350611123031638</v>
+        <v>0.04256964043970326</v>
       </c>
     </row>
     <row r="6">
@@ -597,37 +585,34 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C6" t="n">
-        <v>26.53846153846154</v>
+        <v>26.92307692307692</v>
       </c>
       <c r="D6" t="n">
-        <v>10.55555555555367</v>
+        <v>10.55555555555556</v>
       </c>
       <c r="E6" t="n">
-        <v>8.687719759115941</v>
+        <v>8.018489877597723</v>
       </c>
       <c r="F6" t="n">
-        <v>6.300988610837322</v>
+        <v>0.9315948292169329</v>
       </c>
       <c r="G6" t="n">
-        <v>1.6091945049053</v>
+        <v>2530113.04</v>
       </c>
       <c r="H6" t="n">
-        <v>4261189.58</v>
+        <v>-2.390369806212174</v>
       </c>
       <c r="I6" t="n">
-        <v>-4.15933429851456</v>
+        <v>2715894.25</v>
       </c>
       <c r="J6" t="n">
-        <v>2648026.43</v>
+        <v>23.39922392349369</v>
       </c>
       <c r="K6" t="n">
-        <v>22.90059847107168</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.6214289179783454</v>
+        <v>1.073428027547733</v>
       </c>
     </row>
     <row r="7">
@@ -637,37 +622,34 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C7" t="n">
-        <v>13.46153846153846</v>
+        <v>13.58974358974359</v>
       </c>
       <c r="D7" t="n">
-        <v>9.875000000000242</v>
+        <v>9</v>
       </c>
       <c r="E7" t="n">
-        <v>8.556841380538462</v>
+        <v>7.99742036452254</v>
       </c>
       <c r="F7" t="n">
-        <v>7.331888224468731</v>
+        <v>-7.44741509347587</v>
       </c>
       <c r="G7" t="n">
-        <v>-6.59329065993858</v>
+        <v>-10227832.97</v>
       </c>
       <c r="H7" t="n">
-        <v>-9022474.209999999</v>
+        <v>9.662929176662157</v>
       </c>
       <c r="I7" t="n">
-        <v>8.806809867191138</v>
+        <v>1373339.99</v>
       </c>
       <c r="J7" t="n">
-        <v>1368432.65</v>
+        <v>11.83223166700934</v>
       </c>
       <c r="K7" t="n">
-        <v>11.83444632475008</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.15166933350536</v>
+        <v>0.1342747768787624</v>
       </c>
     </row>
     <row r="8">
@@ -695,40 +677,35 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>weighted_avg_execution_spread_$</t>
+          <t>volume_weighted_avg_spread_in_USD</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>volume_weighted_avg_spread_in_USD</t>
+          <t>PnL_per_lot</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>PnL_per_lot</t>
+          <t>total_profit</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>total_profit</t>
+          <t>pct_total_profit</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>pct_total_profit</t>
+          <t>total_volume</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>total_volume</t>
+          <t>pct_total_volume</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
-        <is>
-          <t>pct_total_volume</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
         <is>
           <t>pct_impact_on_PnL_exec_spread</t>
         </is>
@@ -748,37 +725,34 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="C11" t="n">
-        <v>37.43589743589744</v>
+        <v>38.07692307692307</v>
       </c>
       <c r="D11" t="n">
-        <v>9.306451612902569</v>
+        <v>9.485714285714286</v>
       </c>
       <c r="E11" t="n">
-        <v>11.64637851645355</v>
+        <v>11.74312172667629</v>
       </c>
       <c r="F11" t="n">
-        <v>9.319363923239752</v>
+        <v>-13.93023302051489</v>
       </c>
       <c r="G11" t="n">
-        <v>-7.027145258927329</v>
+        <v>-40300842.67</v>
       </c>
       <c r="H11" t="n">
-        <v>-18830529.4890094</v>
+        <v>39.91742500120819</v>
       </c>
       <c r="I11" t="n">
-        <v>19.32060862060071</v>
+        <v>2893048.71</v>
       </c>
       <c r="J11" t="n">
-        <v>2679684.11</v>
+        <v>41.63687408749787</v>
       </c>
       <c r="K11" t="n">
-        <v>38.8176458546274</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.1423052979770973</v>
+        <v>0.07178630813478223</v>
       </c>
     </row>
     <row r="12">
@@ -788,37 +762,34 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C12" t="n">
-        <v>18.97435897435897</v>
+        <v>18.07692307692308</v>
       </c>
       <c r="D12" t="n">
-        <v>12.03225806451507</v>
+        <v>12.45833333333333</v>
       </c>
       <c r="E12" t="n">
-        <v>12.57051141266667</v>
+        <v>12.83891333892051</v>
       </c>
       <c r="F12" t="n">
-        <v>10.58948804115388</v>
+        <v>-53.15058806449023</v>
       </c>
       <c r="G12" t="n">
-        <v>-41.03899665831257</v>
+        <v>-65625824.09</v>
       </c>
       <c r="H12" t="n">
-        <v>-52182367.9508599</v>
+        <v>65.0014674061667</v>
       </c>
       <c r="I12" t="n">
-        <v>53.54045454022862</v>
+        <v>1234714.92</v>
       </c>
       <c r="J12" t="n">
-        <v>1271531.28</v>
+        <v>17.77006708538793</v>
       </c>
       <c r="K12" t="n">
-        <v>18.41927962177642</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.02436706745844497</v>
+        <v>0.01881446727901958</v>
       </c>
     </row>
     <row r="13">
@@ -834,31 +805,28 @@
         <v>36.53846153846153</v>
       </c>
       <c r="D13" t="n">
-        <v>13.81249999999934</v>
+        <v>13.85714285714286</v>
       </c>
       <c r="E13" t="n">
-        <v>13.38142662346046</v>
+        <v>12.0373041838637</v>
       </c>
       <c r="F13" t="n">
-        <v>10.79304001249265</v>
+        <v>5.863602186952393</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.925120840549116</v>
+        <v>13931578.59</v>
       </c>
       <c r="H13" t="n">
-        <v>-4742705.871906471</v>
+        <v>-13.79903512361874</v>
       </c>
       <c r="I13" t="n">
-        <v>4.866138469829622</v>
+        <v>2375941.98</v>
       </c>
       <c r="J13" t="n">
-        <v>2463588.66</v>
+        <v>34.19465310712324</v>
       </c>
       <c r="K13" t="n">
-        <v>35.68730798472962</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0.5194479114956559</v>
+        <v>0.1705436296864044</v>
       </c>
     </row>
     <row r="14">
@@ -868,37 +836,34 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C14" t="n">
-        <v>7.051282051282051</v>
+        <v>7.307692307692308</v>
       </c>
       <c r="D14" t="n">
-        <v>10.6666666666663</v>
+        <v>10.66666666666667</v>
       </c>
       <c r="E14" t="n">
-        <v>15.26724701789474</v>
+        <v>12.42446739287503</v>
       </c>
       <c r="F14" t="n">
-        <v>11.25885038668071</v>
+        <v>-20.16611088676677</v>
       </c>
       <c r="G14" t="n">
-        <v>-44.44149006024582</v>
+        <v>-8965438.890000001</v>
       </c>
       <c r="H14" t="n">
-        <v>-21707835.12738</v>
+        <v>8.88014271624386</v>
       </c>
       <c r="I14" t="n">
-        <v>22.27279836934104</v>
+        <v>444579.47</v>
       </c>
       <c r="J14" t="n">
-        <v>488458.76</v>
+        <v>6.398405719990982</v>
       </c>
       <c r="K14" t="n">
-        <v>7.07576653886657</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0.02250149575642894</v>
+        <v>0.04958814347570663</v>
       </c>
     </row>
     <row r="15">
@@ -926,40 +891,35 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>weighted_avg_execution_spread_$</t>
+          <t>volume_weighted_avg_spread_in_USD</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>volume_weighted_avg_spread_in_USD</t>
+          <t>PnL_per_lot</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>PnL_per_lot</t>
+          <t>total_profit</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>total_profit</t>
+          <t>pct_total_profit</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>pct_total_profit</t>
+          <t>total_volume</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>total_volume</t>
+          <t>pct_total_volume</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
-        <is>
-          <t>pct_total_volume</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
         <is>
           <t>pct_impact_on_PnL_exec_spread</t>
         </is>
@@ -979,37 +939,34 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>298</v>
+        <v>312</v>
       </c>
       <c r="C18" t="n">
-        <v>38.2051282051282</v>
+        <v>40</v>
       </c>
       <c r="D18" t="n">
-        <v>13.03448275861966</v>
+        <v>12.74626865671642</v>
       </c>
       <c r="E18" t="n">
-        <v>10.23522490275115</v>
+        <v>10.10054608500499</v>
       </c>
       <c r="F18" t="n">
-        <v>8.991338466831536</v>
+        <v>-12.32091114206668</v>
       </c>
       <c r="G18" t="n">
-        <v>-11.84640061832922</v>
+        <v>-13171074.71</v>
       </c>
       <c r="H18" t="n">
-        <v>-11547961</v>
+        <v>30.8260290353123</v>
       </c>
       <c r="I18" t="n">
-        <v>27.92500548563292</v>
+        <v>1069001.68</v>
       </c>
       <c r="J18" t="n">
-        <v>974807.5699999999</v>
+        <v>48.12153104627046</v>
       </c>
       <c r="K18" t="n">
-        <v>44.12544812749606</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0.08441382595594148</v>
+        <v>0.08116282866335665</v>
       </c>
     </row>
     <row r="19">
@@ -1019,37 +976,34 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="C19" t="n">
-        <v>22.56410256410257</v>
+        <v>21.02564102564103</v>
       </c>
       <c r="D19" t="n">
-        <v>13.88461538461494</v>
+        <v>15.05882352941176</v>
       </c>
       <c r="E19" t="n">
-        <v>9.705878733504202</v>
+        <v>9.970005007150476</v>
       </c>
       <c r="F19" t="n">
-        <v>8.734580466490177</v>
+        <v>-43.32202311846592</v>
       </c>
       <c r="G19" t="n">
-        <v>-38.48375812056465</v>
+        <v>-26607183.98</v>
       </c>
       <c r="H19" t="n">
-        <v>-26677650</v>
+        <v>62.27235392512447</v>
       </c>
       <c r="I19" t="n">
-        <v>64.51126069734691</v>
+        <v>614172.24</v>
       </c>
       <c r="J19" t="n">
-        <v>693218.42</v>
+        <v>27.64720492760823</v>
       </c>
       <c r="K19" t="n">
-        <v>31.3790889341727</v>
-      </c>
-      <c r="L19" t="n">
-        <v>0.02598498818299213</v>
+        <v>0.02308294784076582</v>
       </c>
     </row>
     <row r="20">
@@ -1059,37 +1013,34 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C20" t="n">
-        <v>30.38461538461538</v>
+        <v>29.74358974358974</v>
       </c>
       <c r="D20" t="n">
-        <v>13.58333333333064</v>
+        <v>13.41666666666667</v>
       </c>
       <c r="E20" t="n">
-        <v>10.12593069672535</v>
+        <v>9.476296883987487</v>
       </c>
       <c r="F20" t="n">
-        <v>7.638416242373515</v>
+        <v>-3.750660072412065</v>
       </c>
       <c r="G20" t="n">
-        <v>-4.268541113870579</v>
+        <v>-1498636.28</v>
       </c>
       <c r="H20" t="n">
-        <v>-1712438</v>
+        <v>3.507459072081477</v>
       </c>
       <c r="I20" t="n">
-        <v>4.140976969337379</v>
+        <v>399566.01</v>
       </c>
       <c r="J20" t="n">
-        <v>401176.41</v>
+        <v>17.98662108299906</v>
       </c>
       <c r="K20" t="n">
-        <v>18.15957263178628</v>
-      </c>
-      <c r="L20" t="n">
-        <v>0.234272078755552</v>
+        <v>0.2666197364446562</v>
       </c>
     </row>
     <row r="21">
@@ -1099,37 +1050,34 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C21" t="n">
-        <v>8.846153846153847</v>
+        <v>9.230769230769232</v>
       </c>
       <c r="D21" t="n">
-        <v>15.2500000000017</v>
+        <v>16.33333333333333</v>
       </c>
       <c r="E21" t="n">
-        <v>10.3172300865</v>
+        <v>9.561163034961101</v>
       </c>
       <c r="F21" t="n">
-        <v>8.15966777789145</v>
+        <v>-10.45415941867783</v>
       </c>
       <c r="G21" t="n">
-        <v>-10.11231700556952</v>
+        <v>-1450225.98</v>
       </c>
       <c r="H21" t="n">
-        <v>-1415429</v>
+        <v>3.394157967481776</v>
       </c>
       <c r="I21" t="n">
-        <v>3.422756847682799</v>
+        <v>138722.39</v>
       </c>
       <c r="J21" t="n">
-        <v>139970.79</v>
+        <v>6.24464294312226</v>
       </c>
       <c r="K21" t="n">
-        <v>6.335890306544957</v>
-      </c>
-      <c r="L21" t="n">
-        <v>0.09888930493864405</v>
+        <v>0.09565570601624446</v>
       </c>
     </row>
     <row r="22">
@@ -1157,40 +1105,35 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>weighted_avg_execution_spread_$</t>
+          <t>volume_weighted_avg_spread_in_USD</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>volume_weighted_avg_spread_in_USD</t>
+          <t>PnL_per_lot</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>PnL_per_lot</t>
+          <t>total_profit</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>total_profit</t>
+          <t>pct_total_profit</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>pct_total_profit</t>
+          <t>total_volume</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>total_volume</t>
+          <t>pct_total_volume</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
-        <is>
-          <t>pct_total_volume</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
         <is>
           <t>pct_impact_on_PnL_exec_spread</t>
         </is>
@@ -1210,37 +1153,34 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C25" t="n">
-        <v>36.90322580645161</v>
+        <v>36.38709677419355</v>
       </c>
       <c r="D25" t="n">
-        <v>20.56250000000403</v>
+        <v>20.5625</v>
       </c>
       <c r="E25" t="n">
-        <v>27.12954459937888</v>
+        <v>28.07747557994767</v>
       </c>
       <c r="F25" t="n">
-        <v>24.26238381158828</v>
+        <v>-46.60776393818677</v>
       </c>
       <c r="G25" t="n">
-        <v>-45.33398233680204</v>
+        <v>-197392295.31</v>
       </c>
       <c r="H25" t="n">
-        <v>-193105201.01</v>
+        <v>50.02617823322094</v>
       </c>
       <c r="I25" t="n">
-        <v>50.64651425096955</v>
+        <v>4235180.55</v>
       </c>
       <c r="J25" t="n">
-        <v>4259612.57</v>
+        <v>35.44347773516192</v>
       </c>
       <c r="K25" t="n">
-        <v>35.79346966106071</v>
-      </c>
-      <c r="L25" t="n">
-        <v>0.02205850773423454</v>
+        <v>0.02145565278193228</v>
       </c>
     </row>
     <row r="26">
@@ -1250,37 +1190,34 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C26" t="n">
-        <v>17.54838709677419</v>
+        <v>17.03225806451613</v>
       </c>
       <c r="D26" t="n">
-        <v>20.91666666667038</v>
+        <v>20.91666666666667</v>
       </c>
       <c r="E26" t="n">
-        <v>31.58647707173469</v>
+        <v>31.64728689310498</v>
       </c>
       <c r="F26" t="n">
-        <v>29.48027965942457</v>
+        <v>-96.75186500763189</v>
       </c>
       <c r="G26" t="n">
-        <v>-91.28507327936477</v>
+        <v>-234294317.27</v>
       </c>
       <c r="H26" t="n">
-        <v>-228451907.6</v>
+        <v>59.3784537353523</v>
       </c>
       <c r="I26" t="n">
-        <v>59.9170438362528</v>
+        <v>2421600.01</v>
       </c>
       <c r="J26" t="n">
-        <v>2502620.63</v>
+        <v>20.26594262620111</v>
       </c>
       <c r="K26" t="n">
-        <v>21.02948897839543</v>
-      </c>
-      <c r="L26" t="n">
-        <v>0.0109546935120449</v>
+        <v>0.0103357180755236</v>
       </c>
     </row>
     <row r="27">
@@ -1290,37 +1227,34 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C27" t="n">
-        <v>32.12903225806451</v>
+        <v>32.90322580645162</v>
       </c>
       <c r="D27" t="n">
-        <v>21.83783783784071</v>
+        <v>21.83783783783784</v>
       </c>
       <c r="E27" t="n">
-        <v>27.40779447377907</v>
+        <v>27.21979482035463</v>
       </c>
       <c r="F27" t="n">
-        <v>25.00366247890279</v>
+        <v>12.67213012941307</v>
       </c>
       <c r="G27" t="n">
-        <v>13.39790869925987</v>
+        <v>45809245.18</v>
       </c>
       <c r="H27" t="n">
-        <v>47712093.06</v>
+        <v>-11.60968041080325</v>
       </c>
       <c r="I27" t="n">
-        <v>-12.51365156644196</v>
+        <v>3614960.13</v>
       </c>
       <c r="J27" t="n">
-        <v>3561159.74</v>
+        <v>30.2529626230818</v>
       </c>
       <c r="K27" t="n">
-        <v>29.9243795103837</v>
-      </c>
-      <c r="L27" t="n">
-        <v>0.07463851429702925</v>
+        <v>0.07891333104912776</v>
       </c>
     </row>
     <row r="28">
@@ -1330,37 +1264,34 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C28" t="n">
-        <v>13.41935483870968</v>
+        <v>13.67741935483871</v>
       </c>
       <c r="D28" t="n">
-        <v>19.76923076923552</v>
+        <v>19.76923076923077</v>
       </c>
       <c r="E28" t="n">
-        <v>29.91622792105882</v>
+        <v>29.08865352160735</v>
       </c>
       <c r="F28" t="n">
-        <v>27.88272935221994</v>
+        <v>-5.187068883995965</v>
       </c>
       <c r="G28" t="n">
-        <v>-4.714443366140312</v>
+        <v>-8700636.119999999</v>
       </c>
       <c r="H28" t="n">
-        <v>-7435323.02</v>
+        <v>2.205048442230001</v>
       </c>
       <c r="I28" t="n">
-        <v>1.950093479219604</v>
+        <v>1677370.46</v>
       </c>
       <c r="J28" t="n">
-        <v>1577136.99</v>
+        <v>14.03761701555517</v>
       </c>
       <c r="K28" t="n">
-        <v>13.25266185016014</v>
-      </c>
-      <c r="L28" t="n">
-        <v>0.2121141187488046</v>
+        <v>0.192787106237469</v>
       </c>
     </row>
   </sheetData>

</xml_diff>